<commit_message>
login pakai tabel user sipt + validasi update saat import
</commit_message>
<xml_diff>
--- a/datagizi.xlsx
+++ b/datagizi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sipt_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2B4A63-BA11-4A90-B435-F06903C06642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7179A28-1A85-4FDF-8705-1788FBEFE6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7AB274CF-EEAD-49D7-B622-23CC650CDFB0}"/>
   </bookViews>
@@ -1499,7 +1499,7 @@
   <dimension ref="A1:F248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="D2" s="3">
         <f>D3+D4</f>
-        <v>3</v>
+        <v>333335</v>
       </c>
       <c r="E2" s="11"/>
     </row>
@@ -1551,7 +1551,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="5">
-        <v>1</v>
+        <v>333333</v>
       </c>
       <c r="E3" s="11">
         <v>12121212</v>
@@ -1571,7 +1571,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="11">
-        <v>429</v>
+        <v>91919191</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>